<commit_message>
major update for models, especially gropin transfer code update
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema169.xlsx
+++ b/gropin/schema/metadataschema169.xlsx
@@ -632,7 +632,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Gropin Model Nr. 169</t>
+          <t>Gropin growth model for Penicillium expansum in/on Potato Dextrose Agar (gropin ID: 169 )</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>gropinGRT169</t>
+          <t>gropinID169</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Academic Free License 3.0</t>
         </is>
       </c>
     </row>
@@ -5119,17 +5119,17 @@
       </c>
       <c r="P133" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>no idea</t>
         </is>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>dummy unit category</t>
         </is>
       </c>
       <c r="R133" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>Vector[number]</t>
         </is>
       </c>
       <c r="S133" t="inlineStr">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>seq(0.856856,0.981018,length.out=21)</t>
+          <t>seq(0.856,0.982,length.out=21)</t>
         </is>
       </c>
     </row>
@@ -5196,17 +5196,17 @@
       </c>
       <c r="P134" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>no idea</t>
         </is>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>dummy unit category</t>
         </is>
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>Vector[number]</t>
         </is>
       </c>
       <c r="S134" t="inlineStr">
@@ -5226,7 +5226,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>seq(0,0.999,length.out=21)</t>
+          <t>seq(0,1,length.out=21)</t>
         </is>
       </c>
     </row>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>Input</t>
+          <t>Constant</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
@@ -5268,17 +5268,17 @@
       </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>no idea</t>
         </is>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>dummy unit category</t>
         </is>
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>Double</t>
         </is>
       </c>
       <c r="S135" t="inlineStr">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>Input</t>
+          <t>Constant</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
@@ -5340,17 +5340,17 @@
       </c>
       <c r="P136" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>no idea</t>
         </is>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>dummy unit category</t>
         </is>
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>Double</t>
         </is>
       </c>
       <c r="S136" t="inlineStr">

</xml_diff>

<commit_message>
update with all 390 secondary models as fskx files
Signed-off-by: <dr.marcel.fuhrmann@gmail.com>
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema169.xlsx
+++ b/gropin/schema/metadataschema169.xlsx
@@ -984,6 +984,41 @@
           <t>gropinID169</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Marcel</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Fuhrmann</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>BfR</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>marcel.fuhrmann@bfr.bund.de</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>D.</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Judet-Correia</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1016,6 +1051,21 @@
           <t>vCard</t>
         </is>
       </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>S.</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>Bollaert</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1048,6 +1098,21 @@
           <t>vCard</t>
         </is>
       </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>A.</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>Duquenne</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1080,6 +1145,21 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>C.</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>Charpentier</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1102,6 +1182,21 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>M.</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>Bensoussan</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1139,6 +1234,21 @@
           <t>Academic Free License 3.0</t>
         </is>
       </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>P.</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>Dantigny</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1406,6 +1516,31 @@
           <t>RIS</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Judet-Correia,  D.,  Bollaert,  S.,  Duquenne,  A.,  Charpentier,  C.,  Bensoussan,  M.,  Dantigny,  P.</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Validation of a predictive model for the growth of Botrytis cinerea and Penicillium expansum on grape berries</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>International Journal of Food Microbiology ,  142,106-113</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1707,6 +1842,11 @@
           <t>String</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>QRA model</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1824,6 +1964,11 @@
           <t>String</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This model predicts and visualize the mu_max of Penicillium expansum in Potato Dextrose Agar with the independent variable(s) aw according to the publication from Judet-Correia, D., Bollaert, S., Duquenne, A., Charpentier, C., Bensoussan, M., Dantigny, P., 2010 on Validation of a predictive model for the growth of Botrytis cinerea and Penicillium expansum on grape berries. </t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1846,6 +1991,11 @@
           <t>String</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>This model and all metadata included have been automatically generated from the GroPIN microbial modelling DataBase (https://www.aua.gr/psomas/gropin/, version 2020). The model code has been converted from Excel to R and the model itself is provided as an FSKX file. This FSKX model contains also an R script to visualize model-based prediction results similar to those visualizations provided by the GroPIN software. A user of the FSKX model can provide user-defined values for all model input parameters, some of them specifically introduced to customize the generated visualization.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2349,6 +2499,26 @@
           <t>String</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Potato Dextrose Agar</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>none given</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>Penicillium expansum</t>
+        </is>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>log10(CFU)</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5109,22 +5279,22 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>aw</t>
+          <t>water activity</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>descr water activity</t>
         </is>
       </c>
       <c r="P133" t="inlineStr">
         <is>
-          <t>no idea</t>
+          <t>[%]</t>
         </is>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>dummy unit category</t>
+          <t>Dimensionless Parameter</t>
         </is>
       </c>
       <c r="R133" t="inlineStr">
@@ -5132,24 +5302,9 @@
           <t>Vector[number]</t>
         </is>
       </c>
-      <c r="S133" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T133" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U133" t="inlineStr">
-        <is>
-          <t>mydist</t>
-        </is>
-      </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>seq(0.856,0.982,length.out=21)</t>
+          <t>seq(0.855144855144855,0.982982,length.out=21)</t>
         </is>
       </c>
     </row>
@@ -5176,57 +5331,35 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>notused</t>
+          <t>mumax</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>Input</t>
+          <t>Output</t>
         </is>
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>notused</t>
+          <t>data frame with variables and corresponding mumax</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>This dataframe consists of a number of columns 
+                            in relation to the number of variables of this
+                            model. One additional column contains the response
+                            surface mu_max result based on this secondary model.</t>
         </is>
       </c>
       <c r="P134" t="inlineStr">
         <is>
-          <t>no idea</t>
-        </is>
-      </c>
-      <c r="Q134" t="inlineStr">
-        <is>
-          <t>dummy unit category</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>Vector[number]</t>
-        </is>
-      </c>
-      <c r="S134" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T134" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U134" t="inlineStr">
-        <is>
-          <t>mydist</t>
-        </is>
-      </c>
-      <c r="V134" t="inlineStr">
-        <is>
-          <t>seq(0,1,length.out=21)</t>
+          <t>Matrix[number,number]</t>
         </is>
       </c>
     </row>
@@ -5246,59 +5379,9 @@
           <t>0:1</t>
         </is>
       </c>
-      <c r="L135" t="inlineStr">
-        <is>
-          <t>awmin</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr">
-        <is>
-          <t>Constant</t>
-        </is>
-      </c>
-      <c r="N135" t="inlineStr">
-        <is>
-          <t>awmin</t>
-        </is>
-      </c>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>no idea</t>
-        </is>
-      </c>
-      <c r="Q135" t="inlineStr">
-        <is>
-          <t>dummy unit category</t>
-        </is>
-      </c>
-      <c r="R135" t="inlineStr">
-        <is>
-          <t>Double</t>
-        </is>
-      </c>
-      <c r="S135" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T135" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>mydist</t>
-        </is>
-      </c>
-      <c r="V135" t="inlineStr">
-        <is>
-          <t>0.856</t>
+          <t>Add</t>
         </is>
       </c>
     </row>
@@ -5318,59 +5401,9 @@
           <t>0:1</t>
         </is>
       </c>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>awopt</t>
-        </is>
-      </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>Constant</t>
-        </is>
-      </c>
-      <c r="N136" t="inlineStr">
-        <is>
-          <t>awopt</t>
-        </is>
-      </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P136" t="inlineStr">
         <is>
-          <t>no idea</t>
-        </is>
-      </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>dummy unit category</t>
-        </is>
-      </c>
-      <c r="R136" t="inlineStr">
-        <is>
-          <t>Double</t>
-        </is>
-      </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T136" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>mydist</t>
-        </is>
-      </c>
-      <c r="V136" t="inlineStr">
-        <is>
-          <t>0.981</t>
+          <t>Add</t>
         </is>
       </c>
     </row>

</xml_diff>